<commit_message>
optimisation non finie. Commit fait pour premier test de performances entre version 1 et celle-ci
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ion\Desktop\Formation OpClass\Projet4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871240B5-F5C6-405E-9D38-73EBA4F900CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D005E3FC-2021-415B-AAF9-879F64761A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,7 +51,256 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>(SEO ou accessiblité ?)</t>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Le title n'est pas explicite, il empêche google de bien indexer vôtre site</t>
+  </si>
+  <si>
+    <t>Il faut que le title exprime la contenance du site</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>page2.html</t>
+  </si>
+  <si>
+    <t>Lien vers page contact</t>
+  </si>
+  <si>
+    <t>Changer de "page 2&gt;" a "contact"</t>
+  </si>
+  <si>
+    <t>bootstrap.css ligne 7685 &gt; 7926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">et-ligne.css ligne 110 </t>
+  </si>
+  <si>
+    <t>"speak" &gt; speak-as</t>
+  </si>
+  <si>
+    <t>bg : #000/9 &gt; bg : #000</t>
+  </si>
+  <si>
+    <t>Le title n'est pas explicite, l'utilisateur ne sait pas sur quoi il clique</t>
+  </si>
+  <si>
+    <t>Balises html non semantiques</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de balise semantique, il n'y a que des div</t>
+  </si>
+  <si>
+    <t>Il utiliser des balises semantiques pour que google différencie les differentes parties de la page</t>
+  </si>
+  <si>
+    <t>page2.html   ligne 65</t>
+  </si>
+  <si>
+    <t>Sytaxe css incorecte</t>
+  </si>
+  <si>
+    <t>Mots clés cachés</t>
+  </si>
+  <si>
+    <t>lang=default</t>
+  </si>
+  <si>
+    <t>lang=fr</t>
+  </si>
+  <si>
+    <t>index.html et page2.html</t>
+  </si>
+  <si>
+    <t>success-msg et fail-msg</t>
+  </si>
+  <si>
+    <t>data-success-msg et data-fail-msg</t>
+  </si>
+  <si>
+    <t>page2.html ligne 88 et 89</t>
+  </si>
+  <si>
+    <t>min/max-device-width</t>
+  </si>
+  <si>
+    <t>min/max-width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style.css ligne 860 et 866 </t>
+  </si>
+  <si>
+    <t>Il n'y a pas de balise meta, les utilisateurs sont moins guidés quand a la contenance de votre site</t>
+  </si>
+  <si>
+    <t>index.html balise head</t>
+  </si>
+  <si>
+    <t>Le lien vers la 2ème page n'est pas explicite quand a ce qu'elle contient</t>
+  </si>
+  <si>
+    <t>Fournir un maximum d'informations aux utilisateurs pour donner envie de cliquer.</t>
+  </si>
+  <si>
+    <t>Utiliser une balise meta</t>
+  </si>
+  <si>
+    <t>texte img</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>Meta keywords</t>
+  </si>
+  <si>
+    <t>https://constantcontact.com/blog/website-seo-title-tag/</t>
+  </si>
+  <si>
+    <t>n'est plus utilisé par google, bing mais yandex. De plus le mot paris est utilisé alors que l'agence est a lyon</t>
+  </si>
+  <si>
+    <t>https://www.moz.com/learn/seo/meta-description</t>
+  </si>
+  <si>
+    <t>Mettre des noms claires sur les liens pour mieux guider les utilisateurs</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
+  </si>
+  <si>
+    <t>ligne 96, 191, 143</t>
+  </si>
+  <si>
+    <t>https://www.experts-referencement.com/referencement-naturel/black-hat-seo#texte-cache</t>
+  </si>
+  <si>
+    <t>Mots invisibles</t>
+  </si>
+  <si>
+    <t>Mêmes si ce ne sont pas des mots déstinés a tromper les moteurs de recherche google peut l'interpréter ainsi</t>
+  </si>
+  <si>
+    <t>Les textes doivent tous être lisibles</t>
+  </si>
+  <si>
+    <t>page2.html ligne 70 à 76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ahrefs.com/blog/meta-keywords/     </t>
+  </si>
+  <si>
+    <t>Ligne de code</t>
+  </si>
+  <si>
+    <t>https://www.searchenginejournal.com/ranking-factors/meta-keywords/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer les mots clés </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des mots clés sont cachés dans l'attribut alt </t>
+  </si>
+  <si>
+    <t>La balise alt doit expliquer clairement l'image car google interprete ces dernières par la balise alt, de plus cet attribut est lu par les lécteurs d'écran pour les personnes mal voyantes.</t>
+  </si>
+  <si>
+    <t>Accessibilité et SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimiser les images </t>
+  </si>
+  <si>
+    <t>https://www.redacteur.com/blog/referencer-image-sur-google/</t>
+  </si>
+  <si>
+    <t>https://www.redacteur.com/blog/seo-balise-alt-images/</t>
+  </si>
+  <si>
+    <t>La langue du document n'est pas définie</t>
+  </si>
+  <si>
+    <t>Mettre la langue dans laquelle le doc HTML est rédigé</t>
+  </si>
+  <si>
+    <t>https://www.tpgi.com/using-the-html-lang-attribute/</t>
+  </si>
+  <si>
+    <t>https://dequeuniversity.com/rules/axe/3.5/html-has-lang</t>
+  </si>
+  <si>
+    <t>Ecrire le texte sous forme de texte et non sous forme d'image</t>
+  </si>
+  <si>
+    <t>Supprimer l'image et remplacer par du texte</t>
+  </si>
+  <si>
+    <t>Liens non cohérents avec le site et liens cassés</t>
+  </si>
+  <si>
+    <t>Ne mettre que des liens qui fonctionnent pointent vers des sites de qualité</t>
+  </si>
+  <si>
+    <t>Supprimer les liens dans le footer</t>
+  </si>
+  <si>
+    <t>https://www.redacteur.com/blog/seo-liens-penalisant-google/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index.html footer </t>
+  </si>
+  <si>
+    <t>back links dans le footer</t>
+  </si>
+  <si>
+    <t>Mettre les mots clés dans d'autres endroits comme dans un article et les balises alt. Mais ces mots clés doivent être de qualité</t>
+  </si>
+  <si>
+    <t>Supprimer la balise meta</t>
+  </si>
+  <si>
+    <t>Index.html head</t>
+  </si>
+  <si>
+    <t>Mettre un header, un main, une balise footer et des balises articles. Séparer le contenu principal de la page en le mettant dans le main.</t>
+  </si>
+  <si>
+    <t>Changer de "." a "Entreprise web design à Lyon | La Panthère, un design de qualité !"</t>
+  </si>
+  <si>
+    <t>Changer de "page2" a "Contact agence Panthère"</t>
+  </si>
+  <si>
+    <t>Index.html</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr</t>
+  </si>
+  <si>
+    <t>Le crawl du site ne se fera pas correctement, les robots ne liront pas le texte dans l'image mais l'attribut alt de cette image et il y aura donc des pb lors de l'indexation, pareillement pour les lecteurs d'écran. De plus le chargement de la page prendra plus de temps,</t>
+  </si>
+  <si>
+    <t>Images trop volumineuses pouvant ralentir le chargement de la page, balise alt mal utilisée, nom des fichiers image mal utlisé.</t>
+  </si>
+  <si>
+    <t>Uploader des images legères, fournir des bonnes balises alt et nommer les fichiers avec des mots clés pour le référencement</t>
+  </si>
+  <si>
+    <t>convertir les images en .webp, corriger balise alt et changer le nom des fichiers</t>
+  </si>
+  <si>
+    <t>Balise meta description</t>
+  </si>
+  <si>
+    <t>https://blog.horseshoeco.com/getting-backlinks-12-methods-to-use-and-3-to-avoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">index.html header, footer </t>
   </si>
 </sst>
 </file>
@@ -80,17 +329,18 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,8 +353,26 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -119,20 +387,167 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="29">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -346,100 +761,425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="27.5546875" defaultRowHeight="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="27.5546875" defaultRowHeight="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
-    </row>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:26" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:26" ht="158.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F15" r:id="rId1" xr:uid="{7A7D91EE-78C7-4F6D-B897-3DEB975FC899}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{E67C5F9A-BEA5-4CFA-88D8-EFC858D06C50}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{D1F6E7A2-E452-43B5-80C9-0A5479903350}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{B0D9F71C-6D3C-4BD6-964B-28C5EBE285FD}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{2946DD6A-4BAA-4C90-B483-8F71E182EA2B}"/>
+    <hyperlink ref="F11" r:id="rId6" location="texte-cache" xr:uid="{1B5AEC98-0293-4007-AF31-51A6D4BD1702}"/>
+    <hyperlink ref="F16" r:id="rId7" xr:uid="{DAF0E875-B0A7-41D1-A798-3CE46D109992}"/>
+    <hyperlink ref="F17" r:id="rId8" xr:uid="{CC75666D-D8D5-4C84-93A3-00EBC65B4FFD}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{934E8E50-7EF7-4286-A484-4519B9F40965}"/>
+    <hyperlink ref="F8" r:id="rId10" xr:uid="{D2401FCC-48D5-4A36-B042-0C313A45A6F3}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{AA36E9F2-451A-453E-8484-82626A31B4E7}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{3721EC8C-2725-4374-8DBC-BE3DF8600637}"/>
+    <hyperlink ref="F6" r:id="rId13" xr:uid="{9A064156-C23E-4539-B881-3671657DEF52}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>